<commit_message>
changes in stepdefinition file
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Archana Velu\ABN\abn-qa-backend-assingment\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0836C524-9CA4-4E37-AB2B-1C9522161B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A6C73-9FB3-450A-B0B9-50EA9916C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2ADAA468-1DF3-4E56-A8C9-C58D01F65A77}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>TestCase</t>
   </si>
@@ -80,7 +80,16 @@
     <t>issue</t>
   </si>
   <si>
-    <t>create new issue</t>
+    <t xml:space="preserve">create new issue </t>
+  </si>
+  <si>
+    <t>create new issue description</t>
+  </si>
+  <si>
+    <t>regression</t>
+  </si>
+  <si>
+    <t>open</t>
   </si>
 </sst>
 </file>
@@ -483,22 +492,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>1234</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>